<commit_message>
second commit with mail api3
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataFiles/StripeAPITestData.xlsx
+++ b/src/test/resources/testDataFiles/StripeAPITestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\API_Testing_W2A\API_Testing_Framework\RestAssuredAPITestingFramework\src\test\resources\testDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6618715-7753-477C-8438-F6C6C3F4C6B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB849D0-5FBF-490A-9080-B1AFCE408B71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,7 +84,7 @@
     <t>id</t>
   </si>
   <si>
-    <t>cus_GwxvBEhVpO1ewV</t>
+    <t>cus_Gx5PVOskh4zhqb</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>